<commit_message>
Selling ticket routine implementation
</commit_message>
<xml_diff>
--- a/out/production/EventManager/Participants.xlsx
+++ b/out/production/EventManager/Participants.xlsx
@@ -83,7 +83,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -103,6 +103,12 @@
         <v>3</v>
       </c>
     </row>
+    <row r="2">
+      <c r="B2"/>
+      <c r="C2"/>
+      <c r="D2"/>
+      <c r="E2"/>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
Random number for the ticket
</commit_message>
<xml_diff>
--- a/out/production/EventManager/Participants.xlsx
+++ b/out/production/EventManager/Participants.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>First name</t>
   </si>
@@ -24,6 +24,18 @@
   </si>
   <si>
     <t>Ticket type</t>
+  </si>
+  <si>
+    <t>Imad</t>
+  </si>
+  <si>
+    <t>Shehadeh</t>
+  </si>
+  <si>
+    <t>25874125</t>
+  </si>
+  <si>
+    <t>VIP</t>
   </si>
 </sst>
 </file>
@@ -104,10 +116,18 @@
       </c>
     </row>
     <row r="2">
-      <c r="B2"/>
-      <c r="C2"/>
-      <c r="D2"/>
-      <c r="E2"/>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>

</xml_diff>